<commit_message>
fixing bugs on reading excel file
</commit_message>
<xml_diff>
--- a/MultiDirectionCollectionView/initialXLSX.xlsx
+++ b/MultiDirectionCollectionView/initialXLSX.xlsx
@@ -1,25 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27706"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A8E5C4B-EDFD-4A65-96D8-DF9089F81C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{44A9EE0A-384B-419C-A07C-F19575F23623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
-    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
-    <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
-    <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
-    <sheet name="Sheet11" sheetId="11" r:id="rId11"/>
-    <sheet name="Sheet12" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,6 +30,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -410,7 +409,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
@@ -418,134 +419,40 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE3568E-3CEB-462C-8A14-B1B50474D4DF}">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD8F8FF-EF66-4577-B738-DACDB3C46622}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDD78C8A-F96B-4F5F-ACCB-18F91AC9A5CA}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A59E8B9-95C9-4689-99F5-BD1B11974EB5}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8CF263-E96E-4CF5-8A71-FC4C015B4234}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F17448-F217-4D8D-A739-F865CBD028D1}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D609213F-31A3-45C4-89F0-C34FBAF2CBA7}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A76232-5489-47DC-A3EF-507E6A9E5901}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4720D4B3-57E8-49AB-99B5-549A56A42632}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FCB69EB-7A11-46B8-856F-31BCF860756D}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FB50FBE-4B27-409D-A063-60FE711402AA}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3E798FC-7685-49E0-86BB-ACD346D2D11D}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94A6535A-07CA-4FD5-BF18-D98C22A12DE7}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed errors on excelfile reading in icloudviewcontroller
</commit_message>
<xml_diff>
--- a/MultiDirectionCollectionView/initialXLSX.xlsx
+++ b/MultiDirectionCollectionView/initialXLSX.xlsx
@@ -1,16 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27706"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28417"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44A9EE0A-384B-419C-A07C-F19575F23623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2BAD4C7-DDBB-4813-8C26-D75CAD088929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
+    <sheet name="Sheet11" sheetId="11" r:id="rId11"/>
+    <sheet name="Sheet12" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -33,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="1">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -409,9 +418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
@@ -419,13 +426,75 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BEBF4E5-1E70-48B7-ACFB-E1349867504B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35A5559D-329B-4AF7-8B7F-E37C53A29B97}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4807556F-3E46-4302-ABA4-BE882D07BA62}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD8F8FF-EF66-4577-B738-DACDB3C46622}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EF11941-6F89-40E1-9639-31B8E76A8038}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -438,14 +507,134 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A59E8B9-95C9-4689-99F5-BD1B11974EB5}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBF7FDDF-762C-4B28-8A7E-7F7955E72A19}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7E5FBDC-EC53-41DE-A525-4BBA949D0C35}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E4FAF5A-0849-429B-B8F8-E7578035A676}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B466FEF0-D96B-4C6F-8D66-D21235699B98}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C5DAE61-80D7-4243-9A44-2BE1DE8D80AF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B84212ED-2397-4BD8-8DD4-E81AE19CF2F3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF54850-8AA2-432E-A4DD-D8D5DDC619BB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">

</xml_diff>